<commit_message>
un solo programa que hace la funcion de los , envio de mensajes a whatsapp y por medio de correos
</commit_message>
<xml_diff>
--- a/datos_estudiantes_correo.xlsx
+++ b/datos_estudiantes_correo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\send-message\enviar_mensajes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\send-message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E6AA05-A995-463D-A50D-92B9C065BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F9D2C3-465A-470C-B1F4-01BDF056E879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2115" windowWidth="18930" windowHeight="12210" xr2:uid="{055E7051-EFE9-408A-9BBA-8226B2D593B7}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="23385" windowHeight="12210" xr2:uid="{055E7051-EFE9-408A-9BBA-8226B2D593B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
@@ -49,12 +49,24 @@
   <si>
     <t>Correo</t>
   </si>
+  <si>
+    <t>ANALISIS Y DESARROLLO DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>COMPROMISO APRENDIZ SENA, TRATAMIENTO DE DATOS MENOR EDAD(EN CASO DE SER MENOR DE EDAD), DOCUMENTO VIGENTE, TITULO BACHILLER O ACTA DE GRADO, RESULTADOS PRUEBAS ICFES DONDE SE PUEDAN VISUALIZAR SUS DATOS PERSONALES, FOSYGA</t>
+  </si>
+  <si>
+    <t>MARLON</t>
+  </si>
+  <si>
+    <t>kalethsarmiento1234@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +118,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -246,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -298,6 +316,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -636,7 +655,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -661,13 +680,22 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="2"/>
-      <c r="D2" s="18"/>
+      <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="16"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="21"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4">
@@ -756,7 +784,10 @@
       <c r="D20" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{98901B25-BFCC-4CCE-A5B0-926269A9A981}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>